<commit_message>
json files for 1-25 runtime
</commit_message>
<xml_diff>
--- a/mobilenet_v1/build-KV260_SOM/partition_0/deploy/driver/results/excel/runtime_metrics_partition_0.xlsx
+++ b/mobilenet_v1/build-KV260_SOM/partition_0/deploy/driver/results/excel/runtime_metrics_partition_0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,103 +495,173 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>6.442546844482422</v>
+        <v>6.456136703491211</v>
       </c>
       <c r="C2" t="n">
-        <v>155.218118570054</v>
+        <v>154.8913918534658</v>
       </c>
       <c r="D2" t="n">
-        <v>23.36467295211309</v>
+        <v>23.3154914329185</v>
       </c>
       <c r="E2" t="n">
-        <v>31.15289726948412</v>
+        <v>31.087321910558</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06890296936035156</v>
+        <v>0.08320808410644531</v>
       </c>
       <c r="G2" t="n">
-        <v>0.05555152893066406</v>
+        <v>0.06937980651855469</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4286766052246094</v>
+        <v>0.45013427734375</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3094673156738281</v>
+        <v>0.2720355987548828</v>
       </c>
       <c r="J2" t="n">
-        <v>12273.21171760559</v>
+        <v>12211.54141426086</v>
       </c>
       <c r="K2" t="n">
-        <v>0.06532669067382812</v>
+        <v>0.0667572021484375</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>50.34089088439941</v>
+        <v>25.94566345214844</v>
       </c>
       <c r="C3" t="n">
-        <v>198.6456700371782</v>
+        <v>192.7104315224583</v>
       </c>
       <c r="D3" t="n">
-        <v>29.90173541935637</v>
+        <v>29.0083158362126</v>
       </c>
       <c r="E3" t="n">
-        <v>39.86898055914182</v>
+        <v>38.67775444828347</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1070499420166016</v>
+        <v>0.1020431518554688</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08106231689453125</v>
+        <v>0.0820159912109375</v>
       </c>
       <c r="H3" t="n">
-        <v>1.799106597900391</v>
+        <v>1.123428344726562</v>
       </c>
       <c r="I3" t="n">
-        <v>2.535343170166016</v>
+        <v>1.504182815551758</v>
       </c>
       <c r="J3" t="n">
-        <v>257295.1803207397</v>
+        <v>80520.37000656128</v>
       </c>
       <c r="K3" t="n">
-        <v>0.07867813110351562</v>
+        <v>0.06842613220214844</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>50.34089088439941</v>
+      </c>
+      <c r="C4" t="n">
+        <v>198.6456700371782</v>
+      </c>
+      <c r="D4" t="n">
+        <v>29.90173541935637</v>
+      </c>
+      <c r="E4" t="n">
+        <v>39.86898055914182</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.1070499420166016</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.08106231689453125</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.799106597900391</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.535343170166016</v>
+      </c>
+      <c r="J4" t="n">
+        <v>257295.1803207397</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.07867813110351562</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B5" t="n">
+        <v>123.5213279724121</v>
+      </c>
+      <c r="C5" t="n">
+        <v>202.3941971024116</v>
+      </c>
+      <c r="D5" t="n">
+        <v>30.46599370143181</v>
+      </c>
+      <c r="E5" t="n">
+        <v>40.62132493524241</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.1120567321777344</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.08082389831542969</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3.931760787963867</v>
+      </c>
+      <c r="I5" t="n">
+        <v>5.55109977722168</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1318080.536603928</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.07724761962890625</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B6" t="n">
         <v>489.4757270812988</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C6" t="n">
         <v>204.3002225999873</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D6" t="n">
         <v>30.75290390753089</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E6" t="n">
         <v>41.00387187670785</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F6" t="n">
         <v>0.1173019409179688</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G6" t="n">
         <v>0.08249282836914062</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H6" t="n">
         <v>14.51325416564941</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I6" t="n">
         <v>16.8766975402832</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J6" t="n">
         <v>17264854.43377495</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K6" t="n">
         <v>0.06580352783203125</v>
       </c>
     </row>

</xml_diff>